<commit_message>
Base de dados atualizada, funcao que minimiza todas as ligas, tabela com informacoes dos times
</commit_message>
<xml_diff>
--- a/TCL_TURQUIA_2019.xlsx
+++ b/TCL_TURQUIA_2019.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bruno\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65D0094C-8BA5-4DB4-B613-D84F96F8C7F3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81611E1B-00B5-446A-96FC-AF258DB9D0AA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2856" yWindow="2856" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="All Games" sheetId="4" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="13">
   <si>
     <t>Winner</t>
   </si>
@@ -70,9 +70,6 @@
   </si>
   <si>
     <t>AUR</t>
-  </si>
-  <si>
-    <t>BU</t>
   </si>
 </sst>
 </file>
@@ -196,7 +193,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -237,15 +234,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -534,8 +525,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C262"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="E97" sqref="E97"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -668,7 +659,7 @@
       <c r="B12" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="21">
+      <c r="C12" s="8">
         <v>2</v>
       </c>
     </row>
@@ -679,7 +670,7 @@
       <c r="B13" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="20">
+      <c r="C13" s="10">
         <v>2</v>
       </c>
     </row>
@@ -690,7 +681,7 @@
       <c r="B14" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="20">
+      <c r="C14" s="10">
         <v>2</v>
       </c>
     </row>
@@ -701,7 +692,7 @@
       <c r="B15" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="20">
+      <c r="C15" s="10">
         <v>2</v>
       </c>
     </row>
@@ -712,7 +703,7 @@
       <c r="B16" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="20">
+      <c r="C16" s="10">
         <v>2</v>
       </c>
     </row>
@@ -723,7 +714,7 @@
       <c r="B17" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="20">
+      <c r="C17" s="10">
         <v>2</v>
       </c>
     </row>
@@ -734,7 +725,7 @@
       <c r="B18" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="C18" s="20">
+      <c r="C18" s="10">
         <v>2</v>
       </c>
     </row>
@@ -745,7 +736,7 @@
       <c r="B19" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="C19" s="20">
+      <c r="C19" s="10">
         <v>2</v>
       </c>
     </row>
@@ -756,7 +747,7 @@
       <c r="B20" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="C20" s="20">
+      <c r="C20" s="10">
         <v>2</v>
       </c>
     </row>
@@ -767,7 +758,7 @@
       <c r="B21" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C21" s="22">
+      <c r="C21" s="13">
         <v>2</v>
       </c>
     </row>
@@ -778,7 +769,7 @@
       <c r="B22" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="C22" s="21">
+      <c r="C22" s="8">
         <v>3</v>
       </c>
     </row>
@@ -789,7 +780,7 @@
       <c r="B23" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="C23" s="20">
+      <c r="C23" s="10">
         <v>3</v>
       </c>
     </row>
@@ -800,7 +791,7 @@
       <c r="B24" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="C24" s="20">
+      <c r="C24" s="10">
         <v>3</v>
       </c>
     </row>
@@ -811,7 +802,7 @@
       <c r="B25" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="C25" s="20">
+      <c r="C25" s="10">
         <v>3</v>
       </c>
     </row>
@@ -822,7 +813,7 @@
       <c r="B26" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="C26" s="20">
+      <c r="C26" s="10">
         <v>3</v>
       </c>
     </row>
@@ -833,7 +824,7 @@
       <c r="B27" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="C27" s="20">
+      <c r="C27" s="10">
         <v>3</v>
       </c>
     </row>
@@ -844,7 +835,7 @@
       <c r="B28" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="C28" s="20">
+      <c r="C28" s="10">
         <v>3</v>
       </c>
     </row>
@@ -855,7 +846,7 @@
       <c r="B29" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="C29" s="20">
+      <c r="C29" s="10">
         <v>3</v>
       </c>
     </row>
@@ -866,7 +857,7 @@
       <c r="B30" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="C30" s="20">
+      <c r="C30" s="10">
         <v>3</v>
       </c>
     </row>
@@ -877,7 +868,7 @@
       <c r="B31" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C31" s="22">
+      <c r="C31" s="13">
         <v>3</v>
       </c>
     </row>
@@ -888,7 +879,7 @@
       <c r="B32" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="C32" s="21">
+      <c r="C32" s="8">
         <v>4</v>
       </c>
     </row>
@@ -899,7 +890,7 @@
       <c r="B33" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="C33" s="20">
+      <c r="C33" s="10">
         <v>4</v>
       </c>
     </row>
@@ -910,7 +901,7 @@
       <c r="B34" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="C34" s="20">
+      <c r="C34" s="10">
         <v>4</v>
       </c>
     </row>
@@ -921,7 +912,7 @@
       <c r="B35" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="C35" s="20">
+      <c r="C35" s="10">
         <v>4</v>
       </c>
     </row>
@@ -932,7 +923,7 @@
       <c r="B36" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="C36" s="20">
+      <c r="C36" s="10">
         <v>4</v>
       </c>
     </row>
@@ -943,7 +934,7 @@
       <c r="B37" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="C37" s="20">
+      <c r="C37" s="10">
         <v>4</v>
       </c>
     </row>
@@ -954,7 +945,7 @@
       <c r="B38" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="C38" s="20">
+      <c r="C38" s="10">
         <v>4</v>
       </c>
     </row>
@@ -965,7 +956,7 @@
       <c r="B39" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="C39" s="20">
+      <c r="C39" s="10">
         <v>4</v>
       </c>
     </row>
@@ -976,7 +967,7 @@
       <c r="B40" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="C40" s="20">
+      <c r="C40" s="10">
         <v>4</v>
       </c>
     </row>
@@ -987,7 +978,7 @@
       <c r="B41" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C41" s="22">
+      <c r="C41" s="13">
         <v>4</v>
       </c>
     </row>
@@ -998,7 +989,7 @@
       <c r="B42" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="C42" s="21">
+      <c r="C42" s="8">
         <v>5</v>
       </c>
     </row>
@@ -1009,7 +1000,7 @@
       <c r="B43" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="C43" s="20">
+      <c r="C43" s="10">
         <v>5</v>
       </c>
     </row>
@@ -1020,7 +1011,7 @@
       <c r="B44" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="C44" s="20">
+      <c r="C44" s="10">
         <v>5</v>
       </c>
     </row>
@@ -1031,7 +1022,7 @@
       <c r="B45" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="C45" s="20">
+      <c r="C45" s="10">
         <v>5</v>
       </c>
     </row>
@@ -1042,7 +1033,7 @@
       <c r="B46" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="C46" s="20">
+      <c r="C46" s="10">
         <v>5</v>
       </c>
     </row>
@@ -1053,7 +1044,7 @@
       <c r="B47" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="C47" s="20">
+      <c r="C47" s="10">
         <v>5</v>
       </c>
     </row>
@@ -1064,7 +1055,7 @@
       <c r="B48" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="C48" s="20">
+      <c r="C48" s="10">
         <v>5</v>
       </c>
     </row>
@@ -1075,7 +1066,7 @@
       <c r="B49" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="C49" s="20">
+      <c r="C49" s="10">
         <v>5</v>
       </c>
     </row>
@@ -1086,7 +1077,7 @@
       <c r="B50" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="C50" s="20">
+      <c r="C50" s="10">
         <v>5</v>
       </c>
     </row>
@@ -1097,7 +1088,7 @@
       <c r="B51" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C51" s="22">
+      <c r="C51" s="13">
         <v>5</v>
       </c>
     </row>
@@ -1108,7 +1099,7 @@
       <c r="B52" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="C52" s="21">
+      <c r="C52" s="8">
         <v>6</v>
       </c>
     </row>
@@ -1119,7 +1110,7 @@
       <c r="B53" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="C53" s="20">
+      <c r="C53" s="10">
         <v>6</v>
       </c>
     </row>
@@ -1130,7 +1121,7 @@
       <c r="B54" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="C54" s="20">
+      <c r="C54" s="10">
         <v>6</v>
       </c>
     </row>
@@ -1141,18 +1132,18 @@
       <c r="B55" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="C55" s="20">
+      <c r="C55" s="10">
         <v>6</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" s="16" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B56" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="C56" s="20">
+      <c r="C56" s="10">
         <v>6</v>
       </c>
     </row>
@@ -1163,7 +1154,7 @@
       <c r="B57" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="C57" s="20">
+      <c r="C57" s="10">
         <v>6</v>
       </c>
     </row>
@@ -1174,7 +1165,7 @@
       <c r="B58" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="C58" s="20">
+      <c r="C58" s="10">
         <v>6</v>
       </c>
     </row>
@@ -1185,7 +1176,7 @@
       <c r="B59" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="C59" s="20">
+      <c r="C59" s="10">
         <v>6</v>
       </c>
     </row>
@@ -1196,7 +1187,7 @@
       <c r="B60" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="C60" s="20">
+      <c r="C60" s="10">
         <v>6</v>
       </c>
     </row>
@@ -1207,7 +1198,7 @@
       <c r="B61" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C61" s="22">
+      <c r="C61" s="13">
         <v>6</v>
       </c>
     </row>
@@ -1218,7 +1209,7 @@
       <c r="B62" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C62" s="21">
+      <c r="C62" s="8">
         <v>7</v>
       </c>
     </row>
@@ -1226,10 +1217,10 @@
       <c r="A63" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B63" s="19" t="s">
+      <c r="B63" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C63" s="20">
+      <c r="C63" s="10">
         <v>7</v>
       </c>
     </row>
@@ -1237,10 +1228,10 @@
       <c r="A64" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B64" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="C64" s="20">
+      <c r="B64" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C64" s="10">
         <v>7</v>
       </c>
     </row>
@@ -1248,10 +1239,10 @@
       <c r="A65" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B65" s="19" t="s">
+      <c r="B65" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C65" s="20">
+      <c r="C65" s="10">
         <v>7</v>
       </c>
     </row>
@@ -1259,10 +1250,10 @@
       <c r="A66" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B66" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="C66" s="20">
+      <c r="B66" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C66" s="10">
         <v>7</v>
       </c>
     </row>
@@ -1270,10 +1261,10 @@
       <c r="A67" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B67" s="19" t="s">
+      <c r="B67" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C67" s="20">
+      <c r="C67" s="10">
         <v>7</v>
       </c>
     </row>
@@ -1281,10 +1272,10 @@
       <c r="A68" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B68" s="19" t="s">
+      <c r="B68" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C68" s="20">
+      <c r="C68" s="10">
         <v>7</v>
       </c>
     </row>
@@ -1292,10 +1283,10 @@
       <c r="A69" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B69" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="C69" s="20">
+      <c r="B69" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C69" s="10">
         <v>7</v>
       </c>
     </row>
@@ -1303,10 +1294,10 @@
       <c r="A70" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B70" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="C70" s="20">
+      <c r="B70" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C70" s="10">
         <v>7</v>
       </c>
     </row>
@@ -1317,7 +1308,7 @@
       <c r="B71" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C71" s="22">
+      <c r="C71" s="13">
         <v>7</v>
       </c>
     </row>
@@ -1328,7 +1319,7 @@
       <c r="B72" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C72" s="21">
+      <c r="C72" s="8">
         <v>8</v>
       </c>
     </row>
@@ -1336,10 +1327,10 @@
       <c r="A73" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B73" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="C73" s="20">
+      <c r="B73" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C73" s="10">
         <v>8</v>
       </c>
     </row>
@@ -1347,10 +1338,10 @@
       <c r="A74" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B74" s="19" t="s">
+      <c r="B74" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C74" s="20">
+      <c r="C74" s="10">
         <v>8</v>
       </c>
     </row>
@@ -1358,10 +1349,10 @@
       <c r="A75" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B75" s="19" t="s">
+      <c r="B75" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C75" s="20">
+      <c r="C75" s="10">
         <v>8</v>
       </c>
     </row>
@@ -1369,10 +1360,10 @@
       <c r="A76" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B76" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="C76" s="20">
+      <c r="B76" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C76" s="10">
         <v>8</v>
       </c>
     </row>
@@ -1380,10 +1371,10 @@
       <c r="A77" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B77" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="C77" s="20">
+      <c r="B77" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C77" s="10">
         <v>8</v>
       </c>
     </row>
@@ -1391,10 +1382,10 @@
       <c r="A78" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B78" s="19" t="s">
+      <c r="B78" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C78" s="20">
+      <c r="C78" s="10">
         <v>8</v>
       </c>
     </row>
@@ -1402,10 +1393,10 @@
       <c r="A79" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B79" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="C79" s="20">
+      <c r="B79" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C79" s="10">
         <v>8</v>
       </c>
     </row>
@@ -1413,10 +1404,10 @@
       <c r="A80" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B80" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="C80" s="20">
+      <c r="B80" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C80" s="10">
         <v>8</v>
       </c>
     </row>
@@ -1427,7 +1418,7 @@
       <c r="B81" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C81" s="22">
+      <c r="C81" s="13">
         <v>8</v>
       </c>
     </row>
@@ -1438,7 +1429,7 @@
       <c r="B82" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C82" s="21">
+      <c r="C82" s="8">
         <v>9</v>
       </c>
     </row>
@@ -1446,10 +1437,10 @@
       <c r="A83" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B83" s="19" t="s">
+      <c r="B83" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C83" s="20">
+      <c r="C83" s="10">
         <v>9</v>
       </c>
     </row>
@@ -1457,10 +1448,10 @@
       <c r="A84" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B84" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="C84" s="20">
+      <c r="B84" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C84" s="10">
         <v>9</v>
       </c>
     </row>
@@ -1468,10 +1459,10 @@
       <c r="A85" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B85" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="C85" s="20">
+      <c r="B85" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C85" s="10">
         <v>9</v>
       </c>
     </row>
@@ -1479,10 +1470,10 @@
       <c r="A86" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B86" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="C86" s="20">
+      <c r="B86" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C86" s="10">
         <v>9</v>
       </c>
     </row>
@@ -1490,10 +1481,10 @@
       <c r="A87" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B87" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="C87" s="20">
+      <c r="B87" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C87" s="10">
         <v>9</v>
       </c>
     </row>
@@ -1501,10 +1492,10 @@
       <c r="A88" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B88" s="19" t="s">
+      <c r="B88" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C88" s="20">
+      <c r="C88" s="10">
         <v>9</v>
       </c>
     </row>
@@ -1512,10 +1503,10 @@
       <c r="A89" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B89" s="19" t="s">
+      <c r="B89" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C89" s="20">
+      <c r="C89" s="10">
         <v>9</v>
       </c>
     </row>
@@ -1523,10 +1514,10 @@
       <c r="A90" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B90" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="C90" s="20">
+      <c r="B90" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C90" s="10">
         <v>9</v>
       </c>
     </row>
@@ -1534,10 +1525,10 @@
       <c r="A91" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B91" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="C91" s="20">
+      <c r="B91" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C91" s="10">
         <v>9</v>
       </c>
     </row>
@@ -1548,40 +1539,40 @@
       <c r="B92" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C92" s="22">
+      <c r="C92" s="13">
         <v>9</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A93" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="B93" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="C93" s="20">
+      <c r="A93" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B93" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C93" s="10">
         <v>-1</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A94" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="B94" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="C94" s="20">
+      <c r="A94" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B94" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C94" s="10">
         <v>-1</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A95" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="B95" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="C95" s="20">
+      <c r="A95" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B95" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C95" s="10">
         <v>-1</v>
       </c>
     </row>
@@ -1592,7 +1583,7 @@
       <c r="B96" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C96" s="20">
+      <c r="C96" s="10">
         <v>-1</v>
       </c>
     </row>
@@ -1603,7 +1594,7 @@
       <c r="B97" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C97" s="20">
+      <c r="C97" s="10">
         <v>-1</v>
       </c>
     </row>
@@ -1614,7 +1605,7 @@
       <c r="B98" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C98" s="20">
+      <c r="C98" s="10">
         <v>-1</v>
       </c>
     </row>

</xml_diff>